<commit_message>
Updated fitting parameters and ready tu run detail tests.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/10mmolNa2CO3_21C.xlsx
+++ b/Separator Model/Input/10mmolNa2CO3_21C.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Projekte\MA-Model_3\Separator Model\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Projekte\MA-Model_4\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C492818-74FB-4593-B45A-5D077674F7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C959CD60-78F6-41E2-8F42-3577E5DECD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
   </bookViews>
@@ -601,48 +601,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,9 +658,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -698,7 +698,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -804,7 +804,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1100,7 +1100,7 @@
         <v>9.1140000000000006E-3</v>
       </c>
       <c r="K2">
-        <v>0.25330000000000003</v>
+        <v>0.26550000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>